<commit_message>
fix coa cash flow
</commit_message>
<xml_diff>
--- a/storage/template/chart_of_accounts_manufacture.xlsx
+++ b/storage/template/chart_of_accounts_manufacture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martiendt/Projects/Web/point/point/storage/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EF05B3-E005-6F46-93DC-BB98464015A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2596FB-1B1B-3845-87CD-7B9705E59754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1713,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G55" zoomScale="169" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="H62" zoomScale="169" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>